<commit_message>
QoQ_Evaluation First working version
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/2_Evaluation_series/first_release_absolute_GDP.xlsx
+++ b/0_0_Data/2_Processed_Data/2_Evaluation_series/first_release_absolute_GDP.xlsx
@@ -1,40 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,96 +63,38 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -426,992 +382,982 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2">
         <v>34835</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>154.0470106528354</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
+    <row r="3" spans="1:2">
+      <c r="A3" s="2">
         <v>34926</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>154.0266905089688</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
+    <row r="4" spans="1:2">
+      <c r="A4" s="2">
         <v>35018</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>153.6609279193697</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
+    <row r="5" spans="1:2">
+      <c r="A5" s="2">
         <v>35110</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>153.2545250420373</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
+    <row r="6" spans="1:2">
+      <c r="A6" s="2">
         <v>35201</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>155.5710214428318</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
+    <row r="7" spans="1:2">
+      <c r="A7" s="2">
         <v>35292</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>156.8715106502954</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
+    <row r="8" spans="1:2">
+      <c r="A8" s="2">
         <v>35384</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>156.9121509380286</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
+    <row r="9" spans="1:2">
+      <c r="A9" s="2">
         <v>35476</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>157.6030358294937</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
+    <row r="10" spans="1:2">
+      <c r="A10" s="2">
         <v>35566</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>158.436161728025</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
+    <row r="11" spans="1:2">
+      <c r="A11" s="2">
         <v>35657</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>159.6960106477554</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
+    <row r="12" spans="1:2">
+      <c r="A12" s="2">
         <v>35749</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>160.0008128057547</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
+    <row r="13" spans="1:2">
+      <c r="A13" s="2">
         <v>35841</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>161.5654638834843</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="n">
+    <row r="14" spans="1:2">
+      <c r="A14" s="2">
         <v>35931</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>161.4029027325514</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
+    <row r="15" spans="1:2">
+      <c r="A15" s="2">
         <v>36022</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>162.7033919400149</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
+    <row r="16" spans="1:2">
+      <c r="A16" s="2">
         <v>36114</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>161.9921869046833</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="2" t="n">
+    <row r="17" spans="1:2">
+      <c r="A17" s="2">
         <v>36206</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>96.39876250323853</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="2" t="n">
+    <row r="18" spans="1:2">
+      <c r="A18" s="2">
         <v>36296</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>95.93139919430629</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="2" t="n">
+    <row r="19" spans="1:2">
+      <c r="A19" s="2">
         <v>36387</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>96.86612581217075</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="2" t="n">
+    <row r="20" spans="1:2">
+      <c r="A20" s="2">
         <v>36479</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>97.69925171070211</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="2" t="n">
+    <row r="21" spans="1:2">
+      <c r="A21" s="2">
         <v>36571</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>98.29869595476735</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="2" t="n">
+    <row r="22" spans="1:2">
+      <c r="A22" s="2">
         <v>36662</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>99.51993660115113</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="2" t="n">
+    <row r="23" spans="1:2">
+      <c r="A23" s="2">
         <v>36753</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>100.2108214926162</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="2" t="n">
+    <row r="24" spans="1:2">
+      <c r="A24" s="2">
         <v>36845</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>100.302262140016</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="2" t="n">
+    <row r="25" spans="1:2">
+      <c r="A25" s="2">
         <v>36937</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>100.6741207727751</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="2" t="n">
+    <row r="26" spans="1:2">
+      <c r="A26" s="2">
         <v>37027</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>100.8082337222948</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="2" t="n">
+    <row r="27" spans="1:2">
+      <c r="A27" s="2">
         <v>37118</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>100.6659927152284</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="2" t="n">
+    <row r="28" spans="1:2">
+      <c r="A28" s="2">
         <v>37210</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>100.4505991902423</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="2" t="n">
+    <row r="29" spans="1:2">
+      <c r="A29" s="2">
         <v>37302</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>100.6212883987219</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="2" t="n">
+    <row r="30" spans="1:2">
+      <c r="A30" s="2">
         <v>37392</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>100.9850189739343</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="2" t="n">
+    <row r="31" spans="1:2">
+      <c r="A31" s="2">
         <v>37483</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>101.1333560241606</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="2" t="n">
+    <row r="32" spans="1:2">
+      <c r="A32" s="2">
         <v>37575</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>101.1516441536406</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="2" t="n">
+    <row r="33" spans="1:2">
+      <c r="A33" s="2">
         <v>37667</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>100.9220265279478</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="2" t="n">
+    <row r="34" spans="1:2">
+      <c r="A34" s="2">
         <v>37757</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>101.0195632185076</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="2" t="n">
+    <row r="35" spans="1:2">
+      <c r="A35" s="2">
         <v>37848</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>101.1394520673206</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="2" t="n">
+    <row r="36" spans="1:2">
+      <c r="A36" s="2">
         <v>37940</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>101.3365574628268</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="2" t="n">
+    <row r="37" spans="1:2">
+      <c r="A37" s="2">
         <v>38032</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>101.8140808436924</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="2" t="n">
+    <row r="38" spans="1:2">
+      <c r="A38" s="2">
         <v>38123</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>102.2021955915448</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="2" t="n">
+    <row r="39" spans="1:2">
+      <c r="A39" s="2">
         <v>38214</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>102.2408038648914</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="2" t="n">
+    <row r="40" spans="1:2">
+      <c r="A40" s="2">
         <v>38306</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>101.9258416349588</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="2" t="n">
+    <row r="41" spans="1:2">
+      <c r="A41" s="2">
         <v>38398</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>103.55</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="2" t="n">
+    <row r="42" spans="1:2">
+      <c r="A42" s="2">
         <v>38488</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>103.09</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="2" t="n">
+    <row r="43" spans="1:2">
+      <c r="A43" s="2">
         <v>38579</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>103.79</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="2" t="n">
+    <row r="44" spans="1:2">
+      <c r="A44" s="2">
         <v>38671</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>103.9</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="2" t="n">
+    <row r="45" spans="1:2">
+      <c r="A45" s="2">
         <v>38763</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>104.39</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="2" t="n">
+    <row r="46" spans="1:2">
+      <c r="A46" s="2">
         <v>38853</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>105.26</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="2" t="n">
+    <row r="47" spans="1:2">
+      <c r="A47" s="2">
         <v>38944</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>106.24</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="2" t="n">
+    <row r="48" spans="1:2">
+      <c r="A48" s="2">
         <v>39036</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>107.48</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="2" t="n">
+    <row r="49" spans="1:2">
+      <c r="A49" s="2">
         <v>39128</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>108.25</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="2" t="n">
+    <row r="50" spans="1:2">
+      <c r="A50" s="2">
         <v>39218</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>108.27</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="2" t="n">
+    <row r="51" spans="1:2">
+      <c r="A51" s="2">
         <v>39309</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>109.01</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="2" t="n">
+    <row r="52" spans="1:2">
+      <c r="A52" s="2">
         <v>39401</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52">
         <v>109.29</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="2" t="n">
+    <row r="53" spans="1:2">
+      <c r="A53" s="2">
         <v>39493</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>110.96</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" s="2" t="n">
+    <row r="54" spans="1:2">
+      <c r="A54" s="2">
         <v>39584</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54">
         <v>110.39</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" s="2" t="n">
+    <row r="55" spans="1:2">
+      <c r="A55" s="2">
         <v>39675</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55">
         <v>110.02</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="2" t="n">
+    <row r="56" spans="1:2">
+      <c r="A56" s="2">
         <v>39767</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B56">
         <v>107.74</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" s="2" t="n">
+    <row r="57" spans="1:2">
+      <c r="A57" s="2">
         <v>39859</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57">
         <v>103.52</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="2" t="n">
+    <row r="58" spans="1:2">
+      <c r="A58" s="2">
         <v>39949</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58">
         <v>104.26</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="2" t="n">
+    <row r="59" spans="1:2">
+      <c r="A59" s="2">
         <v>40040</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B59">
         <v>105.15</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="2" t="n">
+    <row r="60" spans="1:2">
+      <c r="A60" s="2">
         <v>40132</v>
       </c>
-      <c r="B60" t="n">
+      <c r="B60">
         <v>105.18</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="2" t="n">
+    <row r="61" spans="1:2">
+      <c r="A61" s="2">
         <v>40224</v>
       </c>
-      <c r="B61" t="n">
+      <c r="B61">
         <v>105.53</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="2" t="n">
+    <row r="62" spans="1:2">
+      <c r="A62" s="2">
         <v>40314</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B62">
         <v>108.64</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" s="2" t="n">
+    <row r="63" spans="1:2">
+      <c r="A63" s="2">
         <v>40405</v>
       </c>
-      <c r="B63" t="n">
+      <c r="B63">
         <v>109.64</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="2" t="n">
+    <row r="64" spans="1:2">
+      <c r="A64" s="2">
         <v>40497</v>
       </c>
-      <c r="B64" t="n">
+      <c r="B64">
         <v>110.05</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" s="2" t="n">
+    <row r="65" spans="1:2">
+      <c r="A65" s="2">
         <v>40589</v>
       </c>
-      <c r="B65" t="n">
+      <c r="B65">
         <v>111.71</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" s="2" t="n">
+    <row r="66" spans="1:2">
+      <c r="A66" s="2">
         <v>40679</v>
       </c>
-      <c r="B66" t="n">
+      <c r="B66">
         <v>109.17</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="2" t="n">
+    <row r="67" spans="1:2">
+      <c r="A67" s="2">
         <v>40770</v>
       </c>
-      <c r="B67" t="n">
+      <c r="B67">
         <v>109.89</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" s="2" t="n">
+    <row r="68" spans="1:2">
+      <c r="A68" s="2">
         <v>40862</v>
       </c>
-      <c r="B68" t="n">
+      <c r="B68">
         <v>109.77</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" s="2" t="n">
+    <row r="69" spans="1:2">
+      <c r="A69" s="2">
         <v>40954</v>
       </c>
-      <c r="B69" t="n">
+      <c r="B69">
         <v>110.33</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" s="2" t="n">
+    <row r="70" spans="1:2">
+      <c r="A70" s="2">
         <v>41045</v>
       </c>
-      <c r="B70" t="n">
+      <c r="B70">
         <v>111.12</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" s="2" t="n">
+    <row r="71" spans="1:2">
+      <c r="A71" s="2">
         <v>41136</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B71">
         <v>111.38</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="2" t="n">
+    <row r="72" spans="1:2">
+      <c r="A72" s="2">
         <v>41228</v>
       </c>
-      <c r="B72" t="n">
+      <c r="B72">
         <v>110.73</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" s="2" t="n">
+    <row r="73" spans="1:2">
+      <c r="A73" s="2">
         <v>41320</v>
       </c>
-      <c r="B73" t="n">
+      <c r="B73">
         <v>110.68</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="2" t="n">
+    <row r="74" spans="1:2">
+      <c r="A74" s="2">
         <v>41410</v>
       </c>
-      <c r="B74" t="n">
+      <c r="B74">
         <v>111.69</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" s="2" t="n">
+    <row r="75" spans="1:2">
+      <c r="A75" s="2">
         <v>41501</v>
       </c>
-      <c r="B75" t="n">
+      <c r="B75">
         <v>112.05</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="2" t="n">
+    <row r="76" spans="1:2">
+      <c r="A76" s="2">
         <v>41593</v>
       </c>
-      <c r="B76" t="n">
+      <c r="B76">
         <v>112.48</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="2" t="n">
+    <row r="77" spans="1:2">
+      <c r="A77" s="2">
         <v>41685</v>
       </c>
-      <c r="B77" t="n">
+      <c r="B77">
         <v>113.4</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="2" t="n">
+    <row r="78" spans="1:2">
+      <c r="A78" s="2">
         <v>41775</v>
       </c>
-      <c r="B78" t="n">
+      <c r="B78">
         <v>105.5</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="2" t="n">
+    <row r="79" spans="1:2">
+      <c r="A79" s="2">
         <v>41866</v>
       </c>
-      <c r="B79" t="n">
+      <c r="B79">
         <v>105.75</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="2" t="n">
+    <row r="80" spans="1:2">
+      <c r="A80" s="2">
         <v>41958</v>
       </c>
-      <c r="B80" t="n">
+      <c r="B80">
         <v>106.5</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="2" t="n">
+    <row r="81" spans="1:2">
+      <c r="A81" s="2">
         <v>42050</v>
       </c>
-      <c r="B81" t="n">
+      <c r="B81">
         <v>106.79</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" s="2" t="n">
+    <row r="82" spans="1:2">
+      <c r="A82" s="2">
         <v>42140</v>
       </c>
-      <c r="B82" t="n">
+      <c r="B82">
         <v>107.62</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="2" t="n">
+    <row r="83" spans="1:2">
+      <c r="A83" s="2">
         <v>42231</v>
       </c>
-      <c r="B83" t="n">
+      <c r="B83">
         <v>107.96</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" s="2" t="n">
+    <row r="84" spans="1:2">
+      <c r="A84" s="2">
         <v>42323</v>
       </c>
-      <c r="B84" t="n">
+      <c r="B84">
         <v>108.22</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" s="2" t="n">
+    <row r="85" spans="1:2">
+      <c r="A85" s="2">
         <v>42415</v>
       </c>
-      <c r="B85" t="n">
+      <c r="B85">
         <v>108.94</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="2" t="n">
+    <row r="86" spans="1:2">
+      <c r="A86" s="2">
         <v>42506</v>
       </c>
-      <c r="B86" t="n">
+      <c r="B86">
         <v>109.87</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" s="2" t="n">
+    <row r="87" spans="1:2">
+      <c r="A87" s="2">
         <v>42597</v>
       </c>
-      <c r="B87" t="n">
+      <c r="B87">
         <v>110.08</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="2" t="n">
+    <row r="88" spans="1:2">
+      <c r="A88" s="2">
         <v>42689</v>
       </c>
-      <c r="B88" t="n">
+      <c r="B88">
         <v>110.56</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" s="2" t="n">
+    <row r="89" spans="1:2">
+      <c r="A89" s="2">
         <v>42781</v>
       </c>
-      <c r="B89" t="n">
+      <c r="B89">
         <v>111.25</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" s="2" t="n">
+    <row r="90" spans="1:2">
+      <c r="A90" s="2">
         <v>42871</v>
       </c>
-      <c r="B90" t="n">
+      <c r="B90">
         <v>112.62</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" s="2" t="n">
+    <row r="91" spans="1:2">
+      <c r="A91" s="2">
         <v>42962</v>
       </c>
-      <c r="B91" t="n">
+      <c r="B91">
         <v>113.77</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" s="2" t="n">
+    <row r="92" spans="1:2">
+      <c r="A92" s="2">
         <v>43054</v>
       </c>
-      <c r="B92" t="n">
+      <c r="B92">
         <v>114.37</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" s="2" t="n">
+    <row r="93" spans="1:2">
+      <c r="A93" s="2">
         <v>43146</v>
       </c>
-      <c r="B93" t="n">
+      <c r="B93">
         <v>114.71</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" s="2" t="n">
+    <row r="94" spans="1:2">
+      <c r="A94" s="2">
         <v>43236</v>
       </c>
-      <c r="B94" t="n">
+      <c r="B94">
         <v>115.67</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" s="2" t="n">
+    <row r="95" spans="1:2">
+      <c r="A95" s="2">
         <v>43327</v>
       </c>
-      <c r="B95" t="n">
+      <c r="B95">
         <v>115.44</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" s="2" t="n">
+    <row r="96" spans="1:2">
+      <c r="A96" s="2">
         <v>43419</v>
       </c>
-      <c r="B96" t="n">
+      <c r="B96">
         <v>115.47</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" s="2" t="n">
+    <row r="97" spans="1:2">
+      <c r="A97" s="2">
         <v>43511</v>
       </c>
-      <c r="B97" t="n">
+      <c r="B97">
         <v>115.96</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" s="2" t="n">
+    <row r="98" spans="1:2">
+      <c r="A98" s="2">
         <v>43601</v>
       </c>
-      <c r="B98" t="n">
+      <c r="B98">
         <v>107.03</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" s="2" t="n">
+    <row r="99" spans="1:2">
+      <c r="A99" s="2">
         <v>43692</v>
       </c>
-      <c r="B99" t="n">
+      <c r="B99">
         <v>107.03</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" s="2" t="n">
+    <row r="100" spans="1:2">
+      <c r="A100" s="2">
         <v>43784</v>
       </c>
-      <c r="B100" t="n">
+      <c r="B100">
         <v>107.19</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" s="2" t="n">
+    <row r="101" spans="1:2">
+      <c r="A101" s="2">
         <v>43876</v>
       </c>
-      <c r="B101" t="n">
+      <c r="B101">
         <v>104.74</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" s="2" t="n">
+    <row r="102" spans="1:2">
+      <c r="A102" s="2">
         <v>43967</v>
       </c>
-      <c r="B102" t="n">
+      <c r="B102">
         <v>94.68000000000001</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" s="2" t="n">
+    <row r="103" spans="1:2">
+      <c r="A103" s="2">
         <v>44058</v>
       </c>
-      <c r="B103" t="n">
+      <c r="B103">
         <v>102.72</v>
       </c>
     </row>
-    <row r="104">
-      <c r="A104" s="2" t="n">
+    <row r="104" spans="1:2">
+      <c r="A104" s="2">
         <v>44150</v>
       </c>
-      <c r="B104" t="n">
+      <c r="B104">
         <v>103.1</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" s="2" t="n">
+    <row r="105" spans="1:2">
+      <c r="A105" s="2">
         <v>44242</v>
       </c>
-      <c r="B105" t="n">
+      <c r="B105">
         <v>101.62</v>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" s="2" t="n">
+    <row r="106" spans="1:2">
+      <c r="A106" s="2">
         <v>44332</v>
       </c>
-      <c r="B106" t="n">
+      <c r="B106">
         <v>103.93</v>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" s="2" t="n">
+    <row r="107" spans="1:2">
+      <c r="A107" s="2">
         <v>44423</v>
       </c>
-      <c r="B107" t="n">
+      <c r="B107">
         <v>106.24</v>
       </c>
     </row>
-    <row r="108">
-      <c r="A108" s="2" t="n">
+    <row r="108" spans="1:2">
+      <c r="A108" s="2">
         <v>44515</v>
       </c>
-      <c r="B108" t="n">
+      <c r="B108">
         <v>106.2</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" s="2" t="n">
+    <row r="109" spans="1:2">
+      <c r="A109" s="2">
         <v>44607</v>
       </c>
-      <c r="B109" t="n">
+      <c r="B109">
         <v>106.45</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" s="2" t="n">
+    <row r="110" spans="1:2">
+      <c r="A110" s="2">
         <v>44697</v>
       </c>
-      <c r="B110" t="n">
+      <c r="B110">
         <v>107.5</v>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" s="2" t="n">
+    <row r="111" spans="1:2">
+      <c r="A111" s="2">
         <v>44788</v>
       </c>
-      <c r="B111" t="n">
+      <c r="B111">
         <v>107.89</v>
       </c>
     </row>
-    <row r="112">
-      <c r="A112" s="2" t="n">
+    <row r="112" spans="1:2">
+      <c r="A112" s="2">
         <v>44880</v>
       </c>
-      <c r="B112" t="n">
+      <c r="B112">
         <v>107.5</v>
       </c>
     </row>
-    <row r="113">
-      <c r="A113" s="2" t="n">
+    <row r="113" spans="1:2">
+      <c r="A113" s="2">
         <v>44972</v>
       </c>
-      <c r="B113" t="n">
+      <c r="B113">
         <v>107.03</v>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" s="2" t="n">
+    <row r="114" spans="1:2">
+      <c r="A114" s="2">
         <v>45062</v>
       </c>
-      <c r="B114" t="n">
+      <c r="B114">
         <v>107.78</v>
       </c>
     </row>
-    <row r="115">
-      <c r="A115" s="2" t="n">
+    <row r="115" spans="1:2">
+      <c r="A115" s="2">
         <v>45153</v>
       </c>
-      <c r="B115" t="n">
+      <c r="B115">
         <v>107.87</v>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" s="2" t="n">
+    <row r="116" spans="1:2">
+      <c r="A116" s="2">
         <v>45245</v>
       </c>
-      <c r="B116" t="n">
+      <c r="B116">
         <v>107.68</v>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" s="2" t="n">
+    <row r="117" spans="1:2">
+      <c r="A117" s="2">
         <v>45337</v>
       </c>
-      <c r="B117" t="n">
+      <c r="B117">
         <v>107.91</v>
       </c>
     </row>
-    <row r="118">
-      <c r="A118" s="2" t="n">
+    <row r="118" spans="1:2">
+      <c r="A118" s="2">
         <v>45428</v>
       </c>
-      <c r="B118" t="n">
+      <c r="B118">
         <v>104.78</v>
       </c>
     </row>
-    <row r="119">
-      <c r="A119" s="2" t="n">
+    <row r="119" spans="1:2">
+      <c r="A119" s="2">
         <v>45519</v>
       </c>
-      <c r="B119" t="n">
+      <c r="B119">
         <v>104.66</v>
       </c>
     </row>
-    <row r="120">
-      <c r="A120" s="2" t="n">
+    <row r="120" spans="1:2">
+      <c r="A120" s="2">
         <v>45611</v>
       </c>
-      <c r="B120" t="n">
+      <c r="B120">
         <v>104.45</v>
       </c>
     </row>
-    <row r="121">
-      <c r="A121" s="2" t="n">
+    <row r="121" spans="1:2">
+      <c r="A121" s="2">
         <v>45703</v>
       </c>
-      <c r="B121" t="n">
+      <c r="B121">
         <v>104.88</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Backward extension option fo real-time data
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/2_Evaluation_series/first_release_absolute_GDP.xlsx
+++ b/0_0_Data/2_Processed_Data/2_Evaluation_series/first_release_absolute_GDP.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,961 +399,1305 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>34835</v>
+        <v>30864</v>
       </c>
       <c r="B2">
-        <v>154.0470106528354</v>
+        <v>114.2740640589607</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>34926</v>
+        <v>30956</v>
       </c>
       <c r="B3">
-        <v>154.0266905089688</v>
+        <v>115.2312697283193</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>35018</v>
+        <v>31048</v>
       </c>
       <c r="B4">
-        <v>153.6609279193697</v>
+        <v>114.6202873861755</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>35110</v>
+        <v>31138</v>
       </c>
       <c r="B5">
-        <v>153.2545250420373</v>
+        <v>115.7404216801058</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>35201</v>
+        <v>31229</v>
       </c>
       <c r="B6">
-        <v>155.5710214428318</v>
+        <v>117.2475114573938</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>35292</v>
+        <v>31321</v>
       </c>
       <c r="B7">
-        <v>156.8715106502954</v>
+        <v>117.9603241898949</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>35384</v>
+        <v>31413</v>
       </c>
       <c r="B8">
-        <v>156.9121509380286</v>
+        <v>117.2882436135368</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>35476</v>
+        <v>31503</v>
       </c>
       <c r="B9">
-        <v>157.6030358294937</v>
+        <v>118.6527708443246</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>35566</v>
+        <v>31594</v>
       </c>
       <c r="B10">
-        <v>158.436161728025</v>
+        <v>119.5285122013973</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>35657</v>
+        <v>31686</v>
       </c>
       <c r="B11">
-        <v>159.6960106477554</v>
+        <v>120.709744729542</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>35749</v>
+        <v>31778</v>
       </c>
       <c r="B12">
-        <v>160.0008128057547</v>
+        <v>117.6751990968945</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>35841</v>
+        <v>31868</v>
       </c>
       <c r="B13">
-        <v>161.5654638834843</v>
+        <v>120.3227892461843</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>35931</v>
+        <v>31959</v>
       </c>
       <c r="B14">
-        <v>161.4029027325514</v>
+        <v>121.1781645251856</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>36022</v>
+        <v>32051</v>
       </c>
       <c r="B15">
-        <v>162.7033919400149</v>
+        <v>123.0925758639028</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>36114</v>
+        <v>32143</v>
       </c>
       <c r="B16">
-        <v>161.9921869046833</v>
+        <v>121.992807648044</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>36206</v>
+        <v>32234</v>
       </c>
       <c r="B17">
-        <v>96.39876250323853</v>
+        <v>124.2127101578331</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>36296</v>
+        <v>32325</v>
       </c>
       <c r="B18">
-        <v>95.93139919430629</v>
+        <v>125.5772373886209</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>36387</v>
+        <v>32417</v>
       </c>
       <c r="B19">
-        <v>96.86612581217075</v>
+        <v>127.0843271659089</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>36479</v>
+        <v>32509</v>
       </c>
       <c r="B20">
-        <v>97.69925171070211</v>
+        <v>128.3877561624823</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>36571</v>
+        <v>32599</v>
       </c>
       <c r="B21">
-        <v>98.29869595476735</v>
+        <v>128.9172741923403</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>36662</v>
+        <v>32690</v>
       </c>
       <c r="B22">
-        <v>99.51993660115113</v>
+        <v>130.0781406424135</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>36753</v>
+        <v>32782</v>
       </c>
       <c r="B23">
-        <v>100.2108214926162</v>
+        <v>131.605596497773</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>36845</v>
+        <v>32874</v>
       </c>
       <c r="B24">
-        <v>100.302262140016</v>
+        <v>134.3346509593486</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>36937</v>
+        <v>32964</v>
       </c>
       <c r="B25">
-        <v>100.6741207727751</v>
+        <v>134.9863654576353</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>37027</v>
+        <v>33055</v>
       </c>
       <c r="B26">
-        <v>100.8082337222948</v>
+        <v>137.8376163876397</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>37118</v>
+        <v>33147</v>
       </c>
       <c r="B27">
-        <v>100.6659927152284</v>
+        <v>140.2815457562148</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>37210</v>
+        <v>33239</v>
       </c>
       <c r="B28">
-        <v>100.4505991902423</v>
+        <v>144.1511005897922</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>37302</v>
+        <v>33329</v>
       </c>
       <c r="B29">
-        <v>100.6212883987219</v>
+        <v>145.7563919552551</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
-        <v>37392</v>
+        <v>33420</v>
       </c>
       <c r="B30">
-        <v>100.9850189739343</v>
+        <v>144.8826257689904</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
-        <v>37483</v>
+        <v>33512</v>
       </c>
       <c r="B31">
-        <v>101.1333560241606</v>
+        <v>146.1424746887208</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
-        <v>37575</v>
+        <v>33604</v>
       </c>
       <c r="B32">
-        <v>101.1516441536406</v>
+        <v>148.1135286437828</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
-        <v>37667</v>
+        <v>33695</v>
       </c>
       <c r="B33">
-        <v>100.9220265279478</v>
+        <v>148.0525682121829</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
-        <v>37757</v>
+        <v>33786</v>
       </c>
       <c r="B34">
-        <v>101.0195632185076</v>
+        <v>147.8290466296502</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
-        <v>37848</v>
+        <v>33878</v>
       </c>
       <c r="B35">
-        <v>101.1394520673206</v>
+        <v>147.6258451909839</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
-        <v>37940</v>
+        <v>33970</v>
       </c>
       <c r="B36">
-        <v>101.3365574628268</v>
+        <v>144.9842264883235</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
-        <v>38032</v>
+        <v>34060</v>
       </c>
       <c r="B37">
-        <v>101.8140808436924</v>
+        <v>145.8986329623214</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
-        <v>38123</v>
+        <v>34151</v>
       </c>
       <c r="B38">
-        <v>102.2021955915448</v>
+        <v>146.9552804433855</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
-        <v>38214</v>
+        <v>34243</v>
       </c>
       <c r="B39">
-        <v>102.2408038648914</v>
+        <v>146.6707984292529</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
-        <v>38306</v>
+        <v>34335</v>
       </c>
       <c r="B40">
-        <v>101.9258416349588</v>
+        <v>148.3980106579154</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
-        <v>38398</v>
+        <v>34425</v>
       </c>
       <c r="B41">
-        <v>103.55</v>
+        <v>150.2268236059111</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
-        <v>38488</v>
+        <v>34516</v>
       </c>
       <c r="B42">
-        <v>103.09</v>
+        <v>151.1615502237756</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
-        <v>38579</v>
+        <v>34608</v>
       </c>
       <c r="B43">
-        <v>103.79</v>
+        <v>152.09627684164</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2">
-        <v>38671</v>
+        <v>34700</v>
       </c>
       <c r="B44">
-        <v>103.9</v>
+        <v>152.4213991435059</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2">
-        <v>38763</v>
+        <v>34790</v>
       </c>
       <c r="B45">
-        <v>104.39</v>
+        <v>154.0470106528354</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2">
-        <v>38853</v>
+        <v>34881</v>
       </c>
       <c r="B46">
-        <v>105.26</v>
+        <v>154.0266905089688</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2">
-        <v>38944</v>
+        <v>34973</v>
       </c>
       <c r="B47">
-        <v>106.24</v>
+        <v>153.6609279193697</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2">
-        <v>39036</v>
+        <v>35065</v>
       </c>
       <c r="B48">
-        <v>107.48</v>
+        <v>153.2545250420373</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2">
-        <v>39128</v>
+        <v>35156</v>
       </c>
       <c r="B49">
-        <v>108.25</v>
+        <v>155.5710214428318</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2">
-        <v>39218</v>
+        <v>35247</v>
       </c>
       <c r="B50">
-        <v>108.27</v>
+        <v>156.8715106502954</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2">
-        <v>39309</v>
+        <v>35339</v>
       </c>
       <c r="B51">
-        <v>109.01</v>
+        <v>156.9121509380286</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2">
-        <v>39401</v>
+        <v>35431</v>
       </c>
       <c r="B52">
-        <v>109.29</v>
+        <v>157.6030358294937</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2">
-        <v>39493</v>
+        <v>35521</v>
       </c>
       <c r="B53">
-        <v>110.96</v>
+        <v>158.436161728025</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2">
-        <v>39584</v>
+        <v>35612</v>
       </c>
       <c r="B54">
-        <v>110.39</v>
+        <v>159.6960106477554</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2">
-        <v>39675</v>
+        <v>35704</v>
       </c>
       <c r="B55">
-        <v>110.02</v>
+        <v>160.0008128057547</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2">
-        <v>39767</v>
+        <v>35796</v>
       </c>
       <c r="B56">
-        <v>107.74</v>
+        <v>161.5654638834843</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2">
-        <v>39859</v>
+        <v>35886</v>
       </c>
       <c r="B57">
-        <v>103.52</v>
+        <v>161.4029027325514</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2">
-        <v>39949</v>
+        <v>35977</v>
       </c>
       <c r="B58">
-        <v>104.26</v>
+        <v>162.7033919400149</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2">
-        <v>40040</v>
+        <v>36069</v>
       </c>
       <c r="B59">
-        <v>105.15</v>
+        <v>161.9921869046833</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2">
-        <v>40132</v>
+        <v>36161</v>
       </c>
       <c r="B60">
-        <v>105.18</v>
+        <v>96.39876250323853</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2">
-        <v>40224</v>
+        <v>36251</v>
       </c>
       <c r="B61">
-        <v>105.53</v>
+        <v>95.93139919430629</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2">
-        <v>40314</v>
+        <v>36342</v>
       </c>
       <c r="B62">
-        <v>108.64</v>
+        <v>96.86612581217075</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2">
-        <v>40405</v>
+        <v>36434</v>
       </c>
       <c r="B63">
-        <v>109.64</v>
+        <v>97.69925171070211</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2">
-        <v>40497</v>
+        <v>36526</v>
       </c>
       <c r="B64">
-        <v>110.05</v>
+        <v>98.29869595476735</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2">
-        <v>40589</v>
+        <v>36617</v>
       </c>
       <c r="B65">
-        <v>111.71</v>
+        <v>99.51993660115113</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2">
-        <v>40679</v>
+        <v>36708</v>
       </c>
       <c r="B66">
-        <v>109.17</v>
+        <v>100.2108214926162</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2">
-        <v>40770</v>
+        <v>36800</v>
       </c>
       <c r="B67">
-        <v>109.89</v>
+        <v>100.302262140016</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2">
-        <v>40862</v>
+        <v>36892</v>
       </c>
       <c r="B68">
-        <v>109.77</v>
+        <v>100.6741207727751</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2">
-        <v>40954</v>
+        <v>36982</v>
       </c>
       <c r="B69">
-        <v>110.33</v>
+        <v>100.8082337222948</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2">
-        <v>41045</v>
+        <v>37073</v>
       </c>
       <c r="B70">
-        <v>111.12</v>
+        <v>100.6659927152284</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2">
-        <v>41136</v>
+        <v>37165</v>
       </c>
       <c r="B71">
-        <v>111.38</v>
+        <v>100.4505991902423</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2">
-        <v>41228</v>
+        <v>37257</v>
       </c>
       <c r="B72">
-        <v>110.73</v>
+        <v>100.6212883987219</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2">
-        <v>41320</v>
+        <v>37347</v>
       </c>
       <c r="B73">
-        <v>110.68</v>
+        <v>100.9850189739343</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2">
-        <v>41410</v>
+        <v>37438</v>
       </c>
       <c r="B74">
-        <v>111.69</v>
+        <v>101.1333560241606</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="2">
-        <v>41501</v>
+        <v>37530</v>
       </c>
       <c r="B75">
-        <v>112.05</v>
+        <v>101.1516441536406</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="2">
-        <v>41593</v>
+        <v>37622</v>
       </c>
       <c r="B76">
-        <v>112.48</v>
+        <v>100.9220265279478</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="2">
-        <v>41685</v>
+        <v>37712</v>
       </c>
       <c r="B77">
-        <v>113.4</v>
+        <v>101.0195632185076</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="2">
-        <v>41775</v>
+        <v>37803</v>
       </c>
       <c r="B78">
-        <v>105.5</v>
+        <v>101.1394520673206</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2">
-        <v>41866</v>
+        <v>37895</v>
       </c>
       <c r="B79">
-        <v>105.75</v>
+        <v>101.3365574628268</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="2">
-        <v>41958</v>
+        <v>37987</v>
       </c>
       <c r="B80">
-        <v>106.5</v>
+        <v>101.8140808436924</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2">
-        <v>42050</v>
+        <v>38078</v>
       </c>
       <c r="B81">
-        <v>106.79</v>
+        <v>102.2021955915448</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2">
-        <v>42140</v>
+        <v>38169</v>
       </c>
       <c r="B82">
-        <v>107.62</v>
+        <v>102.2408038648914</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="2">
-        <v>42231</v>
+        <v>38261</v>
       </c>
       <c r="B83">
-        <v>107.96</v>
+        <v>101.9258416349588</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="2">
-        <v>42323</v>
+        <v>38353</v>
       </c>
       <c r="B84">
-        <v>108.22</v>
+        <v>103.55</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="2">
-        <v>42415</v>
+        <v>38443</v>
       </c>
       <c r="B85">
-        <v>108.94</v>
+        <v>103.09</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="2">
-        <v>42506</v>
+        <v>38534</v>
       </c>
       <c r="B86">
-        <v>109.87</v>
+        <v>103.79</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="2">
-        <v>42597</v>
+        <v>38626</v>
       </c>
       <c r="B87">
-        <v>110.08</v>
+        <v>103.9</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="2">
-        <v>42689</v>
+        <v>38718</v>
       </c>
       <c r="B88">
-        <v>110.56</v>
+        <v>104.39</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="2">
-        <v>42781</v>
+        <v>38808</v>
       </c>
       <c r="B89">
-        <v>111.25</v>
+        <v>105.26</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="2">
-        <v>42871</v>
+        <v>38899</v>
       </c>
       <c r="B90">
-        <v>112.62</v>
+        <v>106.24</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="2">
-        <v>42962</v>
+        <v>38991</v>
       </c>
       <c r="B91">
-        <v>113.77</v>
+        <v>107.48</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="2">
-        <v>43054</v>
+        <v>39083</v>
       </c>
       <c r="B92">
-        <v>114.37</v>
+        <v>108.25</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="2">
-        <v>43146</v>
+        <v>39173</v>
       </c>
       <c r="B93">
-        <v>114.71</v>
+        <v>108.27</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="2">
-        <v>43236</v>
+        <v>39264</v>
       </c>
       <c r="B94">
-        <v>115.67</v>
+        <v>109.01</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2">
-        <v>43327</v>
+        <v>39356</v>
       </c>
       <c r="B95">
-        <v>115.44</v>
+        <v>109.29</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="2">
-        <v>43419</v>
+        <v>39448</v>
       </c>
       <c r="B96">
-        <v>115.47</v>
+        <v>110.96</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="2">
-        <v>43511</v>
+        <v>39539</v>
       </c>
       <c r="B97">
-        <v>115.96</v>
+        <v>110.39</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="2">
-        <v>43601</v>
+        <v>39630</v>
       </c>
       <c r="B98">
-        <v>107.03</v>
+        <v>110.02</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="2">
-        <v>43692</v>
+        <v>39722</v>
       </c>
       <c r="B99">
-        <v>107.03</v>
+        <v>107.74</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="2">
-        <v>43784</v>
+        <v>39814</v>
       </c>
       <c r="B100">
-        <v>107.19</v>
+        <v>103.52</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="2">
-        <v>43876</v>
+        <v>39904</v>
       </c>
       <c r="B101">
-        <v>104.74</v>
+        <v>104.26</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="2">
-        <v>43967</v>
+        <v>39995</v>
       </c>
       <c r="B102">
-        <v>94.68000000000001</v>
+        <v>105.15</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="2">
-        <v>44058</v>
+        <v>40087</v>
       </c>
       <c r="B103">
-        <v>102.72</v>
+        <v>105.18</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="2">
-        <v>44150</v>
+        <v>40179</v>
       </c>
       <c r="B104">
-        <v>103.1</v>
+        <v>105.53</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="2">
-        <v>44242</v>
+        <v>40269</v>
       </c>
       <c r="B105">
-        <v>101.62</v>
+        <v>108.64</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="2">
-        <v>44332</v>
+        <v>40360</v>
       </c>
       <c r="B106">
-        <v>103.93</v>
+        <v>109.64</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="2">
-        <v>44423</v>
+        <v>40452</v>
       </c>
       <c r="B107">
-        <v>106.24</v>
+        <v>110.05</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="2">
-        <v>44515</v>
+        <v>40544</v>
       </c>
       <c r="B108">
-        <v>106.2</v>
+        <v>111.71</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="2">
-        <v>44607</v>
+        <v>40634</v>
       </c>
       <c r="B109">
-        <v>106.45</v>
+        <v>109.17</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="2">
-        <v>44697</v>
+        <v>40725</v>
       </c>
       <c r="B110">
-        <v>107.5</v>
+        <v>109.89</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="2">
-        <v>44788</v>
+        <v>40817</v>
       </c>
       <c r="B111">
-        <v>107.89</v>
+        <v>109.77</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="2">
-        <v>44880</v>
+        <v>40909</v>
       </c>
       <c r="B112">
-        <v>107.5</v>
+        <v>110.33</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="2">
-        <v>44972</v>
+        <v>41000</v>
       </c>
       <c r="B113">
-        <v>107.03</v>
+        <v>111.12</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="2">
-        <v>45062</v>
+        <v>41091</v>
       </c>
       <c r="B114">
-        <v>107.78</v>
+        <v>111.38</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="2">
-        <v>45153</v>
+        <v>41183</v>
       </c>
       <c r="B115">
-        <v>107.87</v>
+        <v>110.73</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="2">
-        <v>45245</v>
+        <v>41275</v>
       </c>
       <c r="B116">
-        <v>107.68</v>
+        <v>110.68</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="2">
-        <v>45337</v>
+        <v>41365</v>
       </c>
       <c r="B117">
-        <v>107.91</v>
+        <v>111.69</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="2">
-        <v>45428</v>
+        <v>41456</v>
       </c>
       <c r="B118">
-        <v>104.78</v>
+        <v>112.05</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="2">
-        <v>45519</v>
+        <v>41548</v>
       </c>
       <c r="B119">
-        <v>104.66</v>
+        <v>112.48</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="2">
-        <v>45611</v>
+        <v>41640</v>
       </c>
       <c r="B120">
-        <v>104.45</v>
+        <v>113.4</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="2">
-        <v>45703</v>
+        <v>41730</v>
       </c>
       <c r="B121">
+        <v>105.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="2">
+        <v>41821</v>
+      </c>
+      <c r="B122">
+        <v>105.75</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="2">
+        <v>41913</v>
+      </c>
+      <c r="B123">
+        <v>106.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="2">
+        <v>42005</v>
+      </c>
+      <c r="B124">
+        <v>106.79</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="2">
+        <v>42095</v>
+      </c>
+      <c r="B125">
+        <v>107.62</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="2">
+        <v>42186</v>
+      </c>
+      <c r="B126">
+        <v>107.96</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="2">
+        <v>42278</v>
+      </c>
+      <c r="B127">
+        <v>108.22</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="2">
+        <v>42370</v>
+      </c>
+      <c r="B128">
+        <v>108.94</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="2">
+        <v>42461</v>
+      </c>
+      <c r="B129">
+        <v>109.87</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="2">
+        <v>42552</v>
+      </c>
+      <c r="B130">
+        <v>110.08</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="2">
+        <v>42644</v>
+      </c>
+      <c r="B131">
+        <v>110.56</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="2">
+        <v>42736</v>
+      </c>
+      <c r="B132">
+        <v>111.25</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="2">
+        <v>42826</v>
+      </c>
+      <c r="B133">
+        <v>112.62</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="2">
+        <v>42917</v>
+      </c>
+      <c r="B134">
+        <v>113.77</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="2">
+        <v>43009</v>
+      </c>
+      <c r="B135">
+        <v>114.37</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="2">
+        <v>43101</v>
+      </c>
+      <c r="B136">
+        <v>114.71</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="2">
+        <v>43191</v>
+      </c>
+      <c r="B137">
+        <v>115.67</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="2">
+        <v>43282</v>
+      </c>
+      <c r="B138">
+        <v>115.44</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="2">
+        <v>43374</v>
+      </c>
+      <c r="B139">
+        <v>115.47</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="2">
+        <v>43466</v>
+      </c>
+      <c r="B140">
+        <v>115.96</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="2">
+        <v>43556</v>
+      </c>
+      <c r="B141">
+        <v>107.03</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="2">
+        <v>43647</v>
+      </c>
+      <c r="B142">
+        <v>107.03</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="2">
+        <v>43739</v>
+      </c>
+      <c r="B143">
+        <v>107.19</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="2">
+        <v>43831</v>
+      </c>
+      <c r="B144">
+        <v>104.74</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B145">
+        <v>94.68000000000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B146">
+        <v>102.72</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B147">
+        <v>103.1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B148">
+        <v>101.62</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="2">
+        <v>44287</v>
+      </c>
+      <c r="B149">
+        <v>103.93</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="2">
+        <v>44378</v>
+      </c>
+      <c r="B150">
+        <v>106.24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="2">
+        <v>44470</v>
+      </c>
+      <c r="B151">
+        <v>106.2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="2">
+        <v>44562</v>
+      </c>
+      <c r="B152">
+        <v>106.45</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="2">
+        <v>44652</v>
+      </c>
+      <c r="B153">
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="2">
+        <v>44743</v>
+      </c>
+      <c r="B154">
+        <v>107.89</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="2">
+        <v>44835</v>
+      </c>
+      <c r="B155">
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B156">
+        <v>107.03</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="2">
+        <v>45017</v>
+      </c>
+      <c r="B157">
+        <v>107.78</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="2">
+        <v>45108</v>
+      </c>
+      <c r="B158">
+        <v>107.87</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" s="2">
+        <v>45200</v>
+      </c>
+      <c r="B159">
+        <v>107.68</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" s="2">
+        <v>45292</v>
+      </c>
+      <c r="B160">
+        <v>107.91</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="2">
+        <v>45383</v>
+      </c>
+      <c r="B161">
+        <v>104.78</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" s="2">
+        <v>45474</v>
+      </c>
+      <c r="B162">
+        <v>104.66</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" s="2">
+        <v>45566</v>
+      </c>
+      <c r="B163">
+        <v>104.45</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" s="2">
+        <v>45658</v>
+      </c>
+      <c r="B164">
         <v>104.88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugifixed QoQ Visualizations and a typo in the evaluation objects
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/2_Evaluation_series/first_release_absolute_GDP.xlsx
+++ b/0_0_Data/2_Processed_Data/2_Evaluation_series/first_release_absolute_GDP.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B164"/>
+  <dimension ref="A1:B148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,1305 +399,1177 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>30864</v>
+        <v>32325</v>
       </c>
       <c r="B2">
-        <v>114.2740640589607</v>
+        <v>125.5772373886209</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>30956</v>
+        <v>32417</v>
       </c>
       <c r="B3">
-        <v>115.2312697283193</v>
+        <v>127.0843271659089</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>31048</v>
+        <v>32509</v>
       </c>
       <c r="B4">
-        <v>114.6202873861755</v>
+        <v>128.3877561624823</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>31138</v>
+        <v>32599</v>
       </c>
       <c r="B5">
-        <v>115.7404216801058</v>
+        <v>128.9172741923403</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>31229</v>
+        <v>32690</v>
       </c>
       <c r="B6">
-        <v>117.2475114573938</v>
+        <v>130.0781406424135</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>31321</v>
+        <v>32782</v>
       </c>
       <c r="B7">
-        <v>117.9603241898949</v>
+        <v>131.605596497773</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>31413</v>
+        <v>32874</v>
       </c>
       <c r="B8">
-        <v>117.2882436135368</v>
+        <v>134.3346509593486</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>31503</v>
+        <v>32964</v>
       </c>
       <c r="B9">
-        <v>118.6527708443246</v>
+        <v>134.9863654576353</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>31594</v>
+        <v>33055</v>
       </c>
       <c r="B10">
-        <v>119.5285122013973</v>
+        <v>137.8376163876397</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>31686</v>
+        <v>33147</v>
       </c>
       <c r="B11">
-        <v>120.709744729542</v>
+        <v>140.2815457562148</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>31778</v>
+        <v>33239</v>
       </c>
       <c r="B12">
-        <v>117.6751990968945</v>
+        <v>144.1511005897922</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>31868</v>
+        <v>33329</v>
       </c>
       <c r="B13">
-        <v>120.3227892461843</v>
+        <v>145.7563919552551</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>31959</v>
+        <v>33420</v>
       </c>
       <c r="B14">
-        <v>121.1781645251856</v>
+        <v>144.8826257689904</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>32051</v>
+        <v>33512</v>
       </c>
       <c r="B15">
-        <v>123.0925758639028</v>
+        <v>146.1424746887208</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>32143</v>
+        <v>33604</v>
       </c>
       <c r="B16">
-        <v>121.992807648044</v>
+        <v>148.1135286437828</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>32234</v>
+        <v>33695</v>
       </c>
       <c r="B17">
-        <v>124.2127101578331</v>
+        <v>148.0525682121829</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>32325</v>
+        <v>33786</v>
       </c>
       <c r="B18">
-        <v>125.5772373886209</v>
+        <v>147.8290466296502</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>32417</v>
+        <v>33878</v>
       </c>
       <c r="B19">
-        <v>127.0843271659089</v>
+        <v>147.6258451909839</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>32509</v>
+        <v>33970</v>
       </c>
       <c r="B20">
-        <v>128.3877561624823</v>
+        <v>144.9842264883235</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>32599</v>
+        <v>34060</v>
       </c>
       <c r="B21">
-        <v>128.9172741923403</v>
+        <v>145.8986329623214</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>32690</v>
+        <v>34151</v>
       </c>
       <c r="B22">
-        <v>130.0781406424135</v>
+        <v>146.9552804433855</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>32782</v>
+        <v>34243</v>
       </c>
       <c r="B23">
-        <v>131.605596497773</v>
+        <v>146.6707984292529</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>32874</v>
+        <v>34335</v>
       </c>
       <c r="B24">
-        <v>134.3346509593486</v>
+        <v>148.3980106579154</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>32964</v>
+        <v>34425</v>
       </c>
       <c r="B25">
-        <v>134.9863654576353</v>
+        <v>150.2268236059111</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>33055</v>
+        <v>34516</v>
       </c>
       <c r="B26">
-        <v>137.8376163876397</v>
+        <v>151.1615502237756</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>33147</v>
+        <v>34608</v>
       </c>
       <c r="B27">
-        <v>140.2815457562148</v>
+        <v>152.09627684164</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>33239</v>
+        <v>34700</v>
       </c>
       <c r="B28">
-        <v>144.1511005897922</v>
+        <v>152.4213991435059</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>33329</v>
+        <v>34790</v>
       </c>
       <c r="B29">
-        <v>145.7563919552551</v>
+        <v>154.0470106528354</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
-        <v>33420</v>
+        <v>34881</v>
       </c>
       <c r="B30">
-        <v>144.8826257689904</v>
+        <v>154.0266905089688</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
-        <v>33512</v>
+        <v>34973</v>
       </c>
       <c r="B31">
-        <v>146.1424746887208</v>
+        <v>153.6609279193697</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
-        <v>33604</v>
+        <v>35065</v>
       </c>
       <c r="B32">
-        <v>148.1135286437828</v>
+        <v>153.2545250420373</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
-        <v>33695</v>
+        <v>35156</v>
       </c>
       <c r="B33">
-        <v>148.0525682121829</v>
+        <v>155.5710214428318</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
-        <v>33786</v>
+        <v>35247</v>
       </c>
       <c r="B34">
-        <v>147.8290466296502</v>
+        <v>156.8715106502954</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
-        <v>33878</v>
+        <v>35339</v>
       </c>
       <c r="B35">
-        <v>147.6258451909839</v>
+        <v>156.9121509380286</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
-        <v>33970</v>
+        <v>35431</v>
       </c>
       <c r="B36">
-        <v>144.9842264883235</v>
+        <v>157.6030358294937</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
-        <v>34060</v>
+        <v>35521</v>
       </c>
       <c r="B37">
-        <v>145.8986329623214</v>
+        <v>158.436161728025</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
-        <v>34151</v>
+        <v>35612</v>
       </c>
       <c r="B38">
-        <v>146.9552804433855</v>
+        <v>159.6960106477554</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
-        <v>34243</v>
+        <v>35704</v>
       </c>
       <c r="B39">
-        <v>146.6707984292529</v>
+        <v>160.0008128057547</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
-        <v>34335</v>
+        <v>35796</v>
       </c>
       <c r="B40">
-        <v>148.3980106579154</v>
+        <v>161.5654638834843</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
-        <v>34425</v>
+        <v>35886</v>
       </c>
       <c r="B41">
-        <v>150.2268236059111</v>
+        <v>161.4029027325514</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
-        <v>34516</v>
+        <v>35977</v>
       </c>
       <c r="B42">
-        <v>151.1615502237756</v>
+        <v>162.7033919400149</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
-        <v>34608</v>
+        <v>36069</v>
       </c>
       <c r="B43">
-        <v>152.09627684164</v>
+        <v>161.9921869046833</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2">
-        <v>34700</v>
+        <v>36161</v>
       </c>
       <c r="B44">
-        <v>152.4213991435059</v>
+        <v>96.39876250323853</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2">
-        <v>34790</v>
+        <v>36251</v>
       </c>
       <c r="B45">
-        <v>154.0470106528354</v>
+        <v>95.93139919430629</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2">
-        <v>34881</v>
+        <v>36342</v>
       </c>
       <c r="B46">
-        <v>154.0266905089688</v>
+        <v>96.86612581217075</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2">
-        <v>34973</v>
+        <v>36434</v>
       </c>
       <c r="B47">
-        <v>153.6609279193697</v>
+        <v>97.69925171070211</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2">
-        <v>35065</v>
+        <v>36526</v>
       </c>
       <c r="B48">
-        <v>153.2545250420373</v>
+        <v>98.29869595476735</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2">
-        <v>35156</v>
+        <v>36617</v>
       </c>
       <c r="B49">
-        <v>155.5710214428318</v>
+        <v>99.51993660115113</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2">
-        <v>35247</v>
+        <v>36708</v>
       </c>
       <c r="B50">
-        <v>156.8715106502954</v>
+        <v>100.2108214926162</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2">
-        <v>35339</v>
+        <v>36800</v>
       </c>
       <c r="B51">
-        <v>156.9121509380286</v>
+        <v>100.302262140016</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2">
-        <v>35431</v>
+        <v>36892</v>
       </c>
       <c r="B52">
-        <v>157.6030358294937</v>
+        <v>100.6741207727751</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2">
-        <v>35521</v>
+        <v>36982</v>
       </c>
       <c r="B53">
-        <v>158.436161728025</v>
+        <v>100.8082337222948</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2">
-        <v>35612</v>
+        <v>37073</v>
       </c>
       <c r="B54">
-        <v>159.6960106477554</v>
+        <v>100.6659927152284</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2">
-        <v>35704</v>
+        <v>37165</v>
       </c>
       <c r="B55">
-        <v>160.0008128057547</v>
+        <v>100.4505991902423</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2">
-        <v>35796</v>
+        <v>37257</v>
       </c>
       <c r="B56">
-        <v>161.5654638834843</v>
+        <v>100.6212883987219</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2">
-        <v>35886</v>
+        <v>37347</v>
       </c>
       <c r="B57">
-        <v>161.4029027325514</v>
+        <v>100.9850189739343</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2">
-        <v>35977</v>
+        <v>37438</v>
       </c>
       <c r="B58">
-        <v>162.7033919400149</v>
+        <v>101.1333560241606</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2">
-        <v>36069</v>
+        <v>37530</v>
       </c>
       <c r="B59">
-        <v>161.9921869046833</v>
+        <v>101.1516441536406</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2">
-        <v>36161</v>
+        <v>37622</v>
       </c>
       <c r="B60">
-        <v>96.39876250323853</v>
+        <v>100.9220265279478</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2">
-        <v>36251</v>
+        <v>37712</v>
       </c>
       <c r="B61">
-        <v>95.93139919430629</v>
+        <v>101.0195632185076</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2">
-        <v>36342</v>
+        <v>37803</v>
       </c>
       <c r="B62">
-        <v>96.86612581217075</v>
+        <v>101.1394520673206</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2">
-        <v>36434</v>
+        <v>37895</v>
       </c>
       <c r="B63">
-        <v>97.69925171070211</v>
+        <v>101.3365574628268</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2">
-        <v>36526</v>
+        <v>37987</v>
       </c>
       <c r="B64">
-        <v>98.29869595476735</v>
+        <v>101.8140808436924</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2">
-        <v>36617</v>
+        <v>38078</v>
       </c>
       <c r="B65">
-        <v>99.51993660115113</v>
+        <v>102.2021955915448</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2">
-        <v>36708</v>
+        <v>38169</v>
       </c>
       <c r="B66">
-        <v>100.2108214926162</v>
+        <v>102.2408038648914</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2">
-        <v>36800</v>
+        <v>38261</v>
       </c>
       <c r="B67">
-        <v>100.302262140016</v>
+        <v>101.9258416349588</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2">
-        <v>36892</v>
+        <v>38353</v>
       </c>
       <c r="B68">
-        <v>100.6741207727751</v>
+        <v>103.55</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2">
-        <v>36982</v>
+        <v>38443</v>
       </c>
       <c r="B69">
-        <v>100.8082337222948</v>
+        <v>103.09</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2">
-        <v>37073</v>
+        <v>38534</v>
       </c>
       <c r="B70">
-        <v>100.6659927152284</v>
+        <v>103.79</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2">
-        <v>37165</v>
+        <v>38626</v>
       </c>
       <c r="B71">
-        <v>100.4505991902423</v>
+        <v>103.9</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2">
-        <v>37257</v>
+        <v>38718</v>
       </c>
       <c r="B72">
-        <v>100.6212883987219</v>
+        <v>104.39</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2">
-        <v>37347</v>
+        <v>38808</v>
       </c>
       <c r="B73">
-        <v>100.9850189739343</v>
+        <v>105.26</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2">
-        <v>37438</v>
+        <v>38899</v>
       </c>
       <c r="B74">
-        <v>101.1333560241606</v>
+        <v>106.24</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="2">
-        <v>37530</v>
+        <v>38991</v>
       </c>
       <c r="B75">
-        <v>101.1516441536406</v>
+        <v>107.48</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="2">
-        <v>37622</v>
+        <v>39083</v>
       </c>
       <c r="B76">
-        <v>100.9220265279478</v>
+        <v>108.25</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="2">
-        <v>37712</v>
+        <v>39173</v>
       </c>
       <c r="B77">
-        <v>101.0195632185076</v>
+        <v>108.27</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="2">
-        <v>37803</v>
+        <v>39264</v>
       </c>
       <c r="B78">
-        <v>101.1394520673206</v>
+        <v>109.01</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2">
-        <v>37895</v>
+        <v>39356</v>
       </c>
       <c r="B79">
-        <v>101.3365574628268</v>
+        <v>109.29</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="2">
-        <v>37987</v>
+        <v>39448</v>
       </c>
       <c r="B80">
-        <v>101.8140808436924</v>
+        <v>110.96</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2">
-        <v>38078</v>
+        <v>39539</v>
       </c>
       <c r="B81">
-        <v>102.2021955915448</v>
+        <v>110.39</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2">
-        <v>38169</v>
+        <v>39630</v>
       </c>
       <c r="B82">
-        <v>102.2408038648914</v>
+        <v>110.02</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="2">
-        <v>38261</v>
+        <v>39722</v>
       </c>
       <c r="B83">
-        <v>101.9258416349588</v>
+        <v>107.74</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="2">
-        <v>38353</v>
+        <v>39814</v>
       </c>
       <c r="B84">
-        <v>103.55</v>
+        <v>103.52</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="2">
-        <v>38443</v>
+        <v>39904</v>
       </c>
       <c r="B85">
-        <v>103.09</v>
+        <v>104.26</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="2">
-        <v>38534</v>
+        <v>39995</v>
       </c>
       <c r="B86">
-        <v>103.79</v>
+        <v>105.15</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="2">
-        <v>38626</v>
+        <v>40087</v>
       </c>
       <c r="B87">
-        <v>103.9</v>
+        <v>105.18</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="2">
-        <v>38718</v>
+        <v>40179</v>
       </c>
       <c r="B88">
-        <v>104.39</v>
+        <v>105.53</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="2">
-        <v>38808</v>
+        <v>40269</v>
       </c>
       <c r="B89">
-        <v>105.26</v>
+        <v>108.64</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="2">
-        <v>38899</v>
+        <v>40360</v>
       </c>
       <c r="B90">
-        <v>106.24</v>
+        <v>109.64</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="2">
-        <v>38991</v>
+        <v>40452</v>
       </c>
       <c r="B91">
-        <v>107.48</v>
+        <v>110.05</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="2">
-        <v>39083</v>
+        <v>40544</v>
       </c>
       <c r="B92">
-        <v>108.25</v>
+        <v>111.71</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="2">
-        <v>39173</v>
+        <v>40634</v>
       </c>
       <c r="B93">
-        <v>108.27</v>
+        <v>109.17</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="2">
-        <v>39264</v>
+        <v>40725</v>
       </c>
       <c r="B94">
-        <v>109.01</v>
+        <v>109.89</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2">
-        <v>39356</v>
+        <v>40817</v>
       </c>
       <c r="B95">
-        <v>109.29</v>
+        <v>109.77</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="2">
-        <v>39448</v>
+        <v>40909</v>
       </c>
       <c r="B96">
-        <v>110.96</v>
+        <v>110.33</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="2">
-        <v>39539</v>
+        <v>41000</v>
       </c>
       <c r="B97">
-        <v>110.39</v>
+        <v>111.12</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="2">
-        <v>39630</v>
+        <v>41091</v>
       </c>
       <c r="B98">
-        <v>110.02</v>
+        <v>111.38</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="2">
-        <v>39722</v>
+        <v>41183</v>
       </c>
       <c r="B99">
-        <v>107.74</v>
+        <v>110.73</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="2">
-        <v>39814</v>
+        <v>41275</v>
       </c>
       <c r="B100">
-        <v>103.52</v>
+        <v>110.68</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="2">
-        <v>39904</v>
+        <v>41365</v>
       </c>
       <c r="B101">
-        <v>104.26</v>
+        <v>111.69</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="2">
-        <v>39995</v>
+        <v>41456</v>
       </c>
       <c r="B102">
-        <v>105.15</v>
+        <v>112.05</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="2">
-        <v>40087</v>
+        <v>41548</v>
       </c>
       <c r="B103">
-        <v>105.18</v>
+        <v>112.48</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="2">
-        <v>40179</v>
+        <v>41640</v>
       </c>
       <c r="B104">
-        <v>105.53</v>
+        <v>113.4</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="2">
-        <v>40269</v>
+        <v>41730</v>
       </c>
       <c r="B105">
-        <v>108.64</v>
+        <v>105.5</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="2">
-        <v>40360</v>
+        <v>41821</v>
       </c>
       <c r="B106">
-        <v>109.64</v>
+        <v>105.75</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="2">
-        <v>40452</v>
+        <v>41913</v>
       </c>
       <c r="B107">
-        <v>110.05</v>
+        <v>106.5</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="2">
-        <v>40544</v>
+        <v>42005</v>
       </c>
       <c r="B108">
-        <v>111.71</v>
+        <v>106.79</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="2">
-        <v>40634</v>
+        <v>42095</v>
       </c>
       <c r="B109">
-        <v>109.17</v>
+        <v>107.62</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="2">
-        <v>40725</v>
+        <v>42186</v>
       </c>
       <c r="B110">
-        <v>109.89</v>
+        <v>107.96</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="2">
-        <v>40817</v>
+        <v>42278</v>
       </c>
       <c r="B111">
-        <v>109.77</v>
+        <v>108.22</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="2">
-        <v>40909</v>
+        <v>42370</v>
       </c>
       <c r="B112">
-        <v>110.33</v>
+        <v>108.94</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="2">
-        <v>41000</v>
+        <v>42461</v>
       </c>
       <c r="B113">
-        <v>111.12</v>
+        <v>109.87</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="2">
-        <v>41091</v>
+        <v>42552</v>
       </c>
       <c r="B114">
-        <v>111.38</v>
+        <v>110.08</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="2">
-        <v>41183</v>
+        <v>42644</v>
       </c>
       <c r="B115">
-        <v>110.73</v>
+        <v>110.56</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="2">
-        <v>41275</v>
+        <v>42736</v>
       </c>
       <c r="B116">
-        <v>110.68</v>
+        <v>111.25</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="2">
-        <v>41365</v>
+        <v>42826</v>
       </c>
       <c r="B117">
-        <v>111.69</v>
+        <v>112.62</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="2">
-        <v>41456</v>
+        <v>42917</v>
       </c>
       <c r="B118">
-        <v>112.05</v>
+        <v>113.77</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="2">
-        <v>41548</v>
+        <v>43009</v>
       </c>
       <c r="B119">
-        <v>112.48</v>
+        <v>114.37</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="2">
-        <v>41640</v>
+        <v>43101</v>
       </c>
       <c r="B120">
-        <v>113.4</v>
+        <v>114.71</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="2">
-        <v>41730</v>
+        <v>43191</v>
       </c>
       <c r="B121">
-        <v>105.5</v>
+        <v>115.67</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="2">
-        <v>41821</v>
+        <v>43282</v>
       </c>
       <c r="B122">
-        <v>105.75</v>
+        <v>115.44</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="2">
-        <v>41913</v>
+        <v>43374</v>
       </c>
       <c r="B123">
-        <v>106.5</v>
+        <v>115.47</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="2">
-        <v>42005</v>
+        <v>43466</v>
       </c>
       <c r="B124">
-        <v>106.79</v>
+        <v>115.96</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="2">
-        <v>42095</v>
+        <v>43556</v>
       </c>
       <c r="B125">
-        <v>107.62</v>
+        <v>107.03</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="2">
-        <v>42186</v>
+        <v>43647</v>
       </c>
       <c r="B126">
-        <v>107.96</v>
+        <v>107.03</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="2">
-        <v>42278</v>
+        <v>43739</v>
       </c>
       <c r="B127">
-        <v>108.22</v>
+        <v>107.19</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="2">
-        <v>42370</v>
+        <v>43831</v>
       </c>
       <c r="B128">
-        <v>108.94</v>
+        <v>104.74</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="2">
-        <v>42461</v>
+        <v>43922</v>
       </c>
       <c r="B129">
-        <v>109.87</v>
+        <v>94.68000000000001</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="2">
-        <v>42552</v>
+        <v>44013</v>
       </c>
       <c r="B130">
-        <v>110.08</v>
+        <v>102.72</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="2">
-        <v>42644</v>
+        <v>44105</v>
       </c>
       <c r="B131">
-        <v>110.56</v>
+        <v>103.1</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="2">
-        <v>42736</v>
+        <v>44197</v>
       </c>
       <c r="B132">
-        <v>111.25</v>
+        <v>101.62</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="2">
-        <v>42826</v>
+        <v>44287</v>
       </c>
       <c r="B133">
-        <v>112.62</v>
+        <v>103.93</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="2">
-        <v>42917</v>
+        <v>44378</v>
       </c>
       <c r="B134">
-        <v>113.77</v>
+        <v>106.24</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="2">
-        <v>43009</v>
+        <v>44470</v>
       </c>
       <c r="B135">
-        <v>114.37</v>
+        <v>106.2</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="2">
-        <v>43101</v>
+        <v>44562</v>
       </c>
       <c r="B136">
-        <v>114.71</v>
+        <v>106.45</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="2">
-        <v>43191</v>
+        <v>44652</v>
       </c>
       <c r="B137">
-        <v>115.67</v>
+        <v>107.5</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="2">
-        <v>43282</v>
+        <v>44743</v>
       </c>
       <c r="B138">
-        <v>115.44</v>
+        <v>107.89</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="2">
-        <v>43374</v>
+        <v>44835</v>
       </c>
       <c r="B139">
-        <v>115.47</v>
+        <v>107.5</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="2">
-        <v>43466</v>
+        <v>44927</v>
       </c>
       <c r="B140">
-        <v>115.96</v>
+        <v>107.03</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="2">
-        <v>43556</v>
+        <v>45017</v>
       </c>
       <c r="B141">
-        <v>107.03</v>
+        <v>107.78</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2">
-        <v>43647</v>
+        <v>45108</v>
       </c>
       <c r="B142">
-        <v>107.03</v>
+        <v>107.87</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="2">
-        <v>43739</v>
+        <v>45200</v>
       </c>
       <c r="B143">
-        <v>107.19</v>
+        <v>107.68</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="2">
-        <v>43831</v>
+        <v>45292</v>
       </c>
       <c r="B144">
-        <v>104.74</v>
+        <v>107.91</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="2">
-        <v>43922</v>
+        <v>45383</v>
       </c>
       <c r="B145">
-        <v>94.68000000000001</v>
+        <v>104.78</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="2">
-        <v>44013</v>
+        <v>45474</v>
       </c>
       <c r="B146">
-        <v>102.72</v>
+        <v>104.66</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="2">
-        <v>44105</v>
+        <v>45566</v>
       </c>
       <c r="B147">
-        <v>103.1</v>
+        <v>104.45</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2">
-        <v>44197</v>
+        <v>45658</v>
       </c>
       <c r="B148">
-        <v>101.62</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2">
-      <c r="A149" s="2">
-        <v>44287</v>
-      </c>
-      <c r="B149">
-        <v>103.93</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2">
-      <c r="A150" s="2">
-        <v>44378</v>
-      </c>
-      <c r="B150">
-        <v>106.24</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2">
-      <c r="A151" s="2">
-        <v>44470</v>
-      </c>
-      <c r="B151">
-        <v>106.2</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2">
-      <c r="A152" s="2">
-        <v>44562</v>
-      </c>
-      <c r="B152">
-        <v>106.45</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2">
-      <c r="A153" s="2">
-        <v>44652</v>
-      </c>
-      <c r="B153">
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154" s="2">
-        <v>44743</v>
-      </c>
-      <c r="B154">
-        <v>107.89</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2">
-      <c r="A155" s="2">
-        <v>44835</v>
-      </c>
-      <c r="B155">
-        <v>107.5</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2">
-      <c r="A156" s="2">
-        <v>44927</v>
-      </c>
-      <c r="B156">
-        <v>107.03</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2">
-      <c r="A157" s="2">
-        <v>45017</v>
-      </c>
-      <c r="B157">
-        <v>107.78</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2">
-      <c r="A158" s="2">
-        <v>45108</v>
-      </c>
-      <c r="B158">
-        <v>107.87</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2">
-      <c r="A159" s="2">
-        <v>45200</v>
-      </c>
-      <c r="B159">
-        <v>107.68</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2">
-      <c r="A160" s="2">
-        <v>45292</v>
-      </c>
-      <c r="B160">
-        <v>107.91</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2">
-      <c r="A161" s="2">
-        <v>45383</v>
-      </c>
-      <c r="B161">
-        <v>104.78</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2">
-      <c r="A162" s="2">
-        <v>45474</v>
-      </c>
-      <c r="B162">
-        <v>104.66</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2">
-      <c r="A163" s="2">
-        <v>45566</v>
-      </c>
-      <c r="B163">
-        <v>104.45</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2">
-      <c r="A164" s="2">
-        <v>45658</v>
-      </c>
-      <c r="B164">
         <v>104.88</v>
       </c>
     </row>

</xml_diff>